<commit_message>
Update Cartridge Label Dimensions.xlsx
Updated dimensions
</commit_message>
<xml_diff>
--- a/Cartridge Label Dimensions.xlsx
+++ b/Cartridge Label Dimensions.xlsx
@@ -76,13 +76,13 @@
     <t>Retroflag GPi</t>
   </si>
   <si>
-    <t>22.5 x 40</t>
+    <t>39 x 22</t>
   </si>
   <si>
     <t>Retroflag GPi 2</t>
   </si>
   <si>
-    <t>10 x 40</t>
+    <t>39 x 10</t>
   </si>
   <si>
     <t>Retroflag NESPi 4</t>
@@ -97,7 +97,7 @@
     <t>Sega 32X</t>
   </si>
   <si>
-    <t>75 x 44</t>
+    <t>75 x 43</t>
   </si>
   <si>
     <t>3 (top) 6 (bottom)</t>
@@ -106,7 +106,7 @@
     <t>Sega Genesis</t>
   </si>
   <si>
-    <t>74 x 68</t>
+    <t>74 x 67</t>
   </si>
   <si>
     <t>Sega Genesis Mini</t>

</xml_diff>

<commit_message>
File renames and styles added
General:

-Renamed some files to match their folder name

NES:

-Added publisher styles for Sunsoft, Taxan, Tecmo, Tengen, and Ultra
-Removed Nintendo Seal of Quality logos from the publisher styles, as they're redundant.  From now on they'll all reside at the top level.
</commit_message>
<xml_diff>
--- a/Cartridge Label Dimensions.xlsx
+++ b/Cartridge Label Dimensions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Developer</t>
   </si>
@@ -49,19 +49,31 @@
     <t>90 x 44</t>
   </si>
   <si>
+    <t>Famicom (Large)</t>
+  </si>
+  <si>
+    <t>91 x 67.5</t>
+  </si>
+  <si>
+    <t>Famicom Disk</t>
+  </si>
+  <si>
+    <t>52 x 22</t>
+  </si>
+  <si>
     <t>Gameboy</t>
   </si>
   <si>
     <t>42 x 37</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>Gameboy Advance</t>
   </si>
   <si>
     <t>43 x 22</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>N64</t>
@@ -512,12 +524,10 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="D4" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5">
@@ -533,90 +543,98 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="E6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3">
-        <v>7.0</v>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="3">
         <v>1.0</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3">
         <v>7.0</v>
       </c>
       <c r="E9" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
@@ -625,18 +643,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="D11" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -645,46 +665,40 @@
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -696,7 +710,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>36</v>
@@ -704,113 +718,139 @@
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3">
-        <v>3.5</v>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="3">
         <v>1.0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>2.0</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="D20" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -6708,6 +6748,18 @@
       <c r="E1004" s="4"/>
       <c r="F1004" s="4"/>
     </row>
+    <row r="1005">
+      <c r="C1005" s="4"/>
+      <c r="D1005" s="4"/>
+      <c r="E1005" s="4"/>
+      <c r="F1005" s="4"/>
+    </row>
+    <row r="1006">
+      <c r="C1006" s="4"/>
+      <c r="D1006" s="4"/>
+      <c r="E1006" s="4"/>
+      <c r="F1006" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Spreadsheet and template updates
General:

-Updated spreadsheet with new measurements, and categories for front and rear labels

NES:

-Adjusted corner radius from 1 mm to 1.75 mm
-Added styles for SNK, Mindscape, Milton Bradley, and LJN

SNES:

-Added rear label
-Tweaked colors
-Moved main window down so it's not on the seam any more.  Some games are on the seam, some aren't, so I picked the one that's (to me) more aesthetically pleasing and leaves room above the box for art to "escape"
</commit_message>
<xml_diff>
--- a/Cartridge Label Dimensions.xlsx
+++ b/Cartridge Label Dimensions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>Developer</t>
   </si>
@@ -19,16 +19,16 @@
     <t>System</t>
   </si>
   <si>
-    <t>Dimensions (mm)</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>Back</t>
+    <t>Front/Top (mm)</t>
   </si>
   <si>
     <t>Top Fold (mm)</t>
+  </si>
+  <si>
+    <t>Top (only) (mm)</t>
+  </si>
+  <si>
+    <t>Rear (mm)</t>
   </si>
   <si>
     <t>Corner Radius (mm)</t>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Famicom</t>
@@ -94,25 +97,31 @@
     <t>54.5 x 62.5</t>
   </si>
   <si>
-    <t>4 (top), 3 (bottom), 325 diameter top curve</t>
+    <t>4 (top), 3 (bottom), 325 dia. top curve</t>
   </si>
   <si>
-    <t>NES (Back)</t>
-  </si>
-  <si>
-    <t>NES (Front)</t>
+    <t>NES</t>
   </si>
   <si>
     <t>55 x 97</t>
   </si>
   <si>
-    <t>SNES (Back)</t>
+    <t>x (front only)</t>
   </si>
   <si>
-    <t>SNES (Front)</t>
+    <t>NES (Tengen)</t>
+  </si>
+  <si>
+    <t>SNES</t>
   </si>
   <si>
     <t>82.5 x 44</t>
+  </si>
+  <si>
+    <t>78.5 x 30.5</t>
+  </si>
+  <si>
+    <t>3 (front), 1.5 (rear)</t>
   </si>
   <si>
     <t>Super Famicom</t>
@@ -469,7 +478,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="10.25"/>
     <col customWidth="1" min="2" max="2" width="24.38"/>
-    <col customWidth="1" min="3" max="5" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.88"/>
+    <col customWidth="1" min="5" max="5" width="19.38"/>
+    <col customWidth="1" min="6" max="6" width="17.38"/>
     <col customWidth="1" min="7" max="7" width="32.25"/>
   </cols>
   <sheetData>
@@ -523,11 +534,13 @@
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4">
         <v>1.0</v>
       </c>
@@ -538,16 +551,18 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4">
         <v>1.5</v>
       </c>
@@ -558,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D5" s="4">
+        <v>13.5</v>
+      </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4">
-        <v>13.5</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="3"/>
     </row>
@@ -576,16 +591,18 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="3"/>
     </row>
@@ -594,21 +611,23 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4">
         <v>1.5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -616,21 +635,23 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4">
         <v>1.0</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -638,21 +659,23 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -660,35 +683,37 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12">
@@ -696,235 +721,255 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>36</v>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4">
+        <v>1.0</v>
       </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="4">
         <v>1.0</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="4">
         <v>1.0</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="4"/>
       <c r="G17" s="4">
         <v>1.0</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1.0</v>
+        <v>51</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="D20" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4">
-        <v>7.0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="4"/>
       <c r="G21" s="4">
-        <v>2.0</v>
+        <v>1.25</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -934,12 +979,6 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -8795,14 +8834,6 @@
       <c r="G1005" s="3"/>
       <c r="H1005" s="3"/>
     </row>
-    <row r="1006">
-      <c r="C1006" s="3"/>
-      <c r="D1006" s="3"/>
-      <c r="E1006" s="3"/>
-      <c r="F1006" s="3"/>
-      <c r="G1006" s="3"/>
-      <c r="H1006" s="3"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>